<commit_message>
fixed at risk number
</commit_message>
<xml_diff>
--- a/Burden-of-Illness-Tool/MADMC B19 Pregancy Outcome Estimate Tool.xlsx
+++ b/Burden-of-Illness-Tool/MADMC B19 Pregancy Outcome Estimate Tool.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ritesh/Desktop/parvo-b19-modeling/Phase 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ritesh/Desktop/Scenario-Modeling-of-Human-Parvovirus-B19/Burden-of-Illness-Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A947454-0217-9446-958A-E833D053C911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B370768-1185-CA49-BF20-C051A49EB776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19260" yWindow="660" windowWidth="18980" windowHeight="19020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="20780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -2864,13 +2864,7 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
@@ -2893,32 +2887,20 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2943,6 +2925,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3152,10 +3152,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>18000</c:v>
+                  <c:v>202500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1350</c:v>
+                  <c:v>15187.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3597,6 +3597,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3604,7 +3605,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3818,13 +3818,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-450</c:v>
+                  <c:v>-5062.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-675</c:v>
+                  <c:v>-14175</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>270</c:v>
+                  <c:v>-3037.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3883,13 +3883,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>450</c:v>
+                  <c:v>5062.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1350</c:v>
+                  <c:v>-11137.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-270</c:v>
+                  <c:v>-7087.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6079,8 +6079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4E0B51A-7E99-B445-9709-9B3BD93CABEF}">
   <dimension ref="A1:AC49"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:E13"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6112,25 +6112,25 @@
       <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:29" ht="21" x14ac:dyDescent="0.25">
-      <c r="B4" s="133" t="s">
+      <c r="B4" s="131" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="133"/>
-      <c r="D4" s="133"/>
-      <c r="E4" s="133"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
       <c r="H4" s="100"/>
       <c r="I4" s="33"/>
       <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:29" ht="85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="133"/>
-      <c r="C5" s="133"/>
-      <c r="D5" s="133"/>
-      <c r="E5" s="133"/>
-      <c r="F5" s="133"/>
-      <c r="G5" s="133"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
@@ -6194,17 +6194,17 @@
       <c r="F8" s="32"/>
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="129" t="str">
+      <c r="I8" s="137" t="str">
         <f>_xlfn.CONCAT("Based on ", C9, " pregnancies in the population and historic estimates of parvovirus immunity, mother infection risk, fetal infection risk, and risk of severe fetal outcomes (Table 1), the expected number of severe fetal outcomes due to parvovirus is ",C22,". Under a best case scenario of higher immunity, lower infection rates, and lower complication rates, the number of severe fetal outcomes due to PVB19 could be as low as ", F22, ", while under a worst case scenario the number of severe fetal outcomes may be as high as ", G22, " in the population with ", C9, " pregnancies (Figure 1, Table 2).")</f>
         <v>Based on 3600000 pregnancies in the population and historic estimates of parvovirus immunity, mother infection risk, fetal infection risk, and risk of severe fetal outcomes (Table 1), the expected number of severe fetal outcomes due to parvovirus is . Under a best case scenario of higher immunity, lower infection rates, and lower complication rates, the number of severe fetal outcomes due to PVB19 could be as low as , while under a worst case scenario the number of severe fetal outcomes may be as high as  in the population with 3600000 pregnancies (Figure 1, Table 2).</v>
       </c>
-      <c r="J8" s="129"/>
-      <c r="K8" s="129"/>
-      <c r="L8" s="129"/>
-      <c r="M8" s="129"/>
-      <c r="N8" s="129"/>
-      <c r="O8" s="129"/>
-      <c r="P8" s="129"/>
+      <c r="J8" s="137"/>
+      <c r="K8" s="137"/>
+      <c r="L8" s="137"/>
+      <c r="M8" s="137"/>
+      <c r="N8" s="137"/>
+      <c r="O8" s="137"/>
+      <c r="P8" s="137"/>
       <c r="Q8" s="35"/>
       <c r="R8" s="18"/>
       <c r="X8" s="9"/>
@@ -6231,14 +6231,14 @@
       <c r="F9" s="96"/>
       <c r="G9" s="4"/>
       <c r="H9" s="35"/>
-      <c r="I9" s="129"/>
-      <c r="J9" s="129"/>
-      <c r="K9" s="129"/>
-      <c r="L9" s="129"/>
-      <c r="M9" s="129"/>
-      <c r="N9" s="129"/>
-      <c r="O9" s="129"/>
-      <c r="P9" s="129"/>
+      <c r="I9" s="137"/>
+      <c r="J9" s="137"/>
+      <c r="K9" s="137"/>
+      <c r="L9" s="137"/>
+      <c r="M9" s="137"/>
+      <c r="N9" s="137"/>
+      <c r="O9" s="137"/>
+      <c r="P9" s="137"/>
       <c r="Q9" s="35"/>
       <c r="R9" s="18"/>
       <c r="X9" s="8"/>
@@ -6254,7 +6254,7 @@
         <v>118</v>
       </c>
       <c r="C10" s="72">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D10" s="72">
         <v>0.4</v>
@@ -6265,14 +6265,14 @@
       <c r="F10" s="97"/>
       <c r="G10" s="4"/>
       <c r="H10" s="35"/>
-      <c r="I10" s="129"/>
-      <c r="J10" s="129"/>
-      <c r="K10" s="129"/>
-      <c r="L10" s="129"/>
-      <c r="M10" s="129"/>
-      <c r="N10" s="129"/>
-      <c r="O10" s="129"/>
-      <c r="P10" s="129"/>
+      <c r="I10" s="137"/>
+      <c r="J10" s="137"/>
+      <c r="K10" s="137"/>
+      <c r="L10" s="137"/>
+      <c r="M10" s="137"/>
+      <c r="N10" s="137"/>
+      <c r="O10" s="137"/>
+      <c r="P10" s="137"/>
       <c r="Q10" s="35"/>
       <c r="R10" s="18"/>
       <c r="X10" s="8"/>
@@ -6288,7 +6288,7 @@
         <v>119</v>
       </c>
       <c r="C11" s="72">
-        <v>0.01</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="D11" s="72">
         <v>5.0000000000000001E-3</v>
@@ -6352,12 +6352,12 @@
     </row>
     <row r="13" spans="1:29" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="B13" s="134" t="s">
+      <c r="B13" s="132" t="s">
         <v>121</v>
       </c>
-      <c r="C13" s="134"/>
-      <c r="D13" s="134"/>
-      <c r="E13" s="134"/>
+      <c r="C13" s="132"/>
+      <c r="D13" s="132"/>
+      <c r="E13" s="132"/>
       <c r="F13" s="97"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -6436,20 +6436,20 @@
     </row>
     <row r="17" spans="1:18" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="135" t="s">
+      <c r="B17" s="133" t="s">
         <v>100</v>
       </c>
       <c r="C17" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="137" t="s">
+      <c r="D17" s="135" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="138"/>
-      <c r="F17" s="137" t="s">
+      <c r="E17" s="136"/>
+      <c r="F17" s="135" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="138"/>
+      <c r="G17" s="136"/>
       <c r="H17" s="101"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -6464,7 +6464,7 @@
     </row>
     <row r="18" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="136"/>
+      <c r="B18" s="134"/>
       <c r="C18" s="111" t="s">
         <v>41</v>
       </c>
@@ -6498,8 +6498,8 @@
         <v>122</v>
       </c>
       <c r="C19" s="114">
-        <f>C9*C10</f>
-        <v>1800000</v>
+        <f>C9-(C9*C10)</f>
+        <v>2700000</v>
       </c>
       <c r="D19" s="115">
         <f>C9-(D10*C9)</f>
@@ -6536,15 +6536,15 @@
       </c>
       <c r="C20" s="57">
         <f>C19*C11</f>
-        <v>18000</v>
+        <v>202500</v>
       </c>
       <c r="D20" s="116">
         <f>D19*C11</f>
-        <v>21600</v>
+        <v>162000</v>
       </c>
       <c r="E20" s="102">
         <f t="shared" ref="E20:G21" si="0">E19*C11</f>
-        <v>14400</v>
+        <v>108000</v>
       </c>
       <c r="F20" s="102">
         <f t="shared" si="0"/>
@@ -6573,15 +6573,15 @@
       </c>
       <c r="C21" s="57">
         <f>C20*C12</f>
-        <v>1350</v>
+        <v>15187.5</v>
       </c>
       <c r="D21" s="116">
         <f>D20*C12</f>
-        <v>1620</v>
+        <v>12150</v>
       </c>
       <c r="E21" s="102">
         <f t="shared" si="0"/>
-        <v>1080</v>
+        <v>8100</v>
       </c>
       <c r="F21" s="102">
         <f t="shared" si="0"/>
@@ -6649,14 +6649,14 @@
     </row>
     <row r="24" spans="1:18" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
-      <c r="B24" s="132" t="s">
+      <c r="B24" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="132"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="132"/>
-      <c r="F24" s="132"/>
-      <c r="G24" s="132"/>
+      <c r="C24" s="130"/>
+      <c r="D24" s="130"/>
+      <c r="E24" s="130"/>
+      <c r="F24" s="130"/>
+      <c r="G24" s="130"/>
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="3"/>
@@ -6671,14 +6671,14 @@
     </row>
     <row r="25" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
-      <c r="B25" s="132" t="s">
+      <c r="B25" s="130" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="132"/>
-      <c r="D25" s="132"/>
-      <c r="E25" s="132"/>
-      <c r="F25" s="132"/>
-      <c r="G25" s="132"/>
+      <c r="C25" s="130"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="130"/>
       <c r="H25" s="40"/>
       <c r="I25" s="46"/>
       <c r="J25" s="99"/>
@@ -6915,14 +6915,14 @@
     </row>
     <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
-      <c r="B37" s="131" t="s">
+      <c r="B37" s="138" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="131"/>
-      <c r="D37" s="131"/>
-      <c r="E37" s="131"/>
-      <c r="F37" s="131"/>
-      <c r="G37" s="131"/>
+      <c r="C37" s="138"/>
+      <c r="D37" s="138"/>
+      <c r="E37" s="138"/>
+      <c r="F37" s="138"/>
+      <c r="G37" s="138"/>
       <c r="H37" s="3"/>
       <c r="I37" s="38"/>
       <c r="J37" s="3"/>
@@ -6937,14 +6937,14 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
-      <c r="B38" s="130" t="s">
+      <c r="B38" s="129" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="130"/>
-      <c r="D38" s="130"/>
-      <c r="E38" s="130"/>
-      <c r="F38" s="130"/>
-      <c r="G38" s="130"/>
+      <c r="C38" s="129"/>
+      <c r="D38" s="129"/>
+      <c r="E38" s="129"/>
+      <c r="F38" s="129"/>
+      <c r="G38" s="129"/>
       <c r="H38" s="35"/>
       <c r="I38" s="36"/>
       <c r="J38" s="3"/>
@@ -6959,14 +6959,14 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
-      <c r="B39" s="130" t="s">
+      <c r="B39" s="129" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="130"/>
-      <c r="D39" s="130"/>
-      <c r="E39" s="130"/>
-      <c r="F39" s="130"/>
-      <c r="G39" s="130"/>
+      <c r="C39" s="129"/>
+      <c r="D39" s="129"/>
+      <c r="E39" s="129"/>
+      <c r="F39" s="129"/>
+      <c r="G39" s="129"/>
       <c r="H39" s="35"/>
       <c r="I39" s="36"/>
       <c r="J39" s="3"/>
@@ -6981,14 +6981,14 @@
     </row>
     <row r="40" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
-      <c r="B40" s="130" t="s">
+      <c r="B40" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="130"/>
-      <c r="D40" s="130"/>
-      <c r="E40" s="130"/>
-      <c r="F40" s="130"/>
-      <c r="G40" s="130"/>
+      <c r="C40" s="129"/>
+      <c r="D40" s="129"/>
+      <c r="E40" s="129"/>
+      <c r="F40" s="129"/>
+      <c r="G40" s="129"/>
       <c r="H40" s="35"/>
       <c r="I40" s="36"/>
       <c r="J40" s="3"/>
@@ -7003,14 +7003,14 @@
     </row>
     <row r="41" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
-      <c r="B41" s="130" t="s">
+      <c r="B41" s="129" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="130"/>
-      <c r="D41" s="130"/>
-      <c r="E41" s="130"/>
-      <c r="F41" s="130"/>
-      <c r="G41" s="130"/>
+      <c r="C41" s="129"/>
+      <c r="D41" s="129"/>
+      <c r="E41" s="129"/>
+      <c r="F41" s="129"/>
+      <c r="G41" s="129"/>
       <c r="H41" s="35"/>
       <c r="I41" s="36"/>
       <c r="J41" s="3"/>
@@ -7079,23 +7079,23 @@
       </c>
       <c r="C47" s="43">
         <f>F47-E47</f>
-        <v>-450</v>
+        <v>-5062.5</v>
       </c>
       <c r="D47" s="43">
         <f>G47-E47</f>
-        <v>450</v>
+        <v>5062.5</v>
       </c>
       <c r="E47" s="43">
         <f>C21</f>
-        <v>1350</v>
+        <v>15187.5</v>
       </c>
       <c r="F47" s="1">
         <f>C20*D12</f>
-        <v>900</v>
+        <v>10125</v>
       </c>
       <c r="G47" s="1">
         <f>C20*E12</f>
-        <v>1800</v>
+        <v>20250</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="48" x14ac:dyDescent="0.2">
@@ -7104,23 +7104,23 @@
       </c>
       <c r="C48" s="43">
         <f>F48-E48</f>
-        <v>-675</v>
+        <v>-14175</v>
       </c>
       <c r="D48" s="43">
         <f>G48-E48</f>
-        <v>1350</v>
+        <v>-11137.5</v>
       </c>
       <c r="E48" s="43">
         <f>C21</f>
-        <v>1350</v>
+        <v>15187.5</v>
       </c>
       <c r="F48" s="1">
         <f>(C9-(C9*C10))*D11*C12</f>
-        <v>675</v>
+        <v>1012.5</v>
       </c>
       <c r="G48" s="1">
         <f>(C9-(C9*C10))*E11*C12</f>
-        <v>2700</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="49" spans="2:7" ht="32" x14ac:dyDescent="0.2">
@@ -7129,27 +7129,32 @@
       </c>
       <c r="C49" s="43">
         <f>F49-E49</f>
-        <v>270</v>
+        <v>-3037.5</v>
       </c>
       <c r="D49" s="43">
         <f>G49-E49</f>
-        <v>-270</v>
+        <v>-7087.5</v>
       </c>
       <c r="E49" s="43">
         <f>C21</f>
-        <v>1350</v>
+        <v>15187.5</v>
       </c>
       <c r="F49" s="1">
         <f>(C9-(C9*D10))*C11*C12</f>
-        <v>1620</v>
+        <v>12150</v>
       </c>
       <c r="G49" s="1">
         <f>(C9-(C9*E10))*C11*C12</f>
-        <v>1080</v>
+        <v>8100</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="I8:P10"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
     <mergeCell ref="B41:G41"/>
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="B25:G25"/>
@@ -7158,11 +7163,6 @@
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="F17:G17"/>
-    <mergeCell ref="I8:P10"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -7174,8 +7174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A54D747-3B89-BC41-8182-1F289A700DB3}">
   <dimension ref="B1:AH128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7217,25 +7217,25 @@
       <c r="F2" s="7"/>
     </row>
     <row r="3" spans="2:34" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="146" t="s">
+      <c r="C3" s="139" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="146"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
-      <c r="H3" s="146"/>
-      <c r="I3" s="146"/>
-      <c r="J3" s="146"/>
-      <c r="K3" s="146"/>
-      <c r="L3" s="146"/>
-      <c r="M3" s="146"/>
-      <c r="N3" s="146"/>
-      <c r="O3" s="146"/>
-      <c r="P3" s="146"/>
-      <c r="Q3" s="146"/>
-      <c r="R3" s="146"/>
-      <c r="S3" s="146"/>
+      <c r="D3" s="139"/>
+      <c r="E3" s="139"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="139"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="139"/>
+      <c r="K3" s="139"/>
+      <c r="L3" s="139"/>
+      <c r="M3" s="139"/>
+      <c r="N3" s="139"/>
+      <c r="O3" s="139"/>
+      <c r="P3" s="139"/>
+      <c r="Q3" s="139"/>
+      <c r="R3" s="139"/>
+      <c r="S3" s="139"/>
     </row>
     <row r="6" spans="2:34" ht="26.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
@@ -7247,20 +7247,20 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="147" t="str">
+      <c r="I6" s="140" t="str">
         <f>_xlfn.CONCAT("Figure 1. Estimated Number of Severe Fetal Outcomes Under Potential Immunity and Infection Rate Scenarios, based on ",D8," Pregnancies")</f>
         <v>Figure 1. Estimated Number of Severe Fetal Outcomes Under Potential Immunity and Infection Rate Scenarios, based on 3600000 Pregnancies</v>
       </c>
-      <c r="J6" s="147"/>
-      <c r="K6" s="147"/>
-      <c r="L6" s="147"/>
-      <c r="M6" s="147"/>
-      <c r="N6" s="147"/>
-      <c r="O6" s="147"/>
-      <c r="P6" s="147"/>
-      <c r="Q6" s="147"/>
-      <c r="R6" s="147"/>
-      <c r="S6" s="147"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="140"/>
+      <c r="L6" s="140"/>
+      <c r="M6" s="140"/>
+      <c r="N6" s="140"/>
+      <c r="O6" s="140"/>
+      <c r="P6" s="140"/>
+      <c r="Q6" s="140"/>
+      <c r="R6" s="140"/>
+      <c r="S6" s="140"/>
       <c r="T6" s="3"/>
       <c r="W6" s="54" t="s">
         <v>22</v>
@@ -7281,17 +7281,17 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="147"/>
-      <c r="J7" s="147"/>
-      <c r="K7" s="147"/>
-      <c r="L7" s="147"/>
-      <c r="M7" s="147"/>
-      <c r="N7" s="147"/>
-      <c r="O7" s="147"/>
-      <c r="P7" s="147"/>
-      <c r="Q7" s="147"/>
-      <c r="R7" s="147"/>
-      <c r="S7" s="147"/>
+      <c r="I7" s="140"/>
+      <c r="J7" s="140"/>
+      <c r="K7" s="140"/>
+      <c r="L7" s="140"/>
+      <c r="M7" s="140"/>
+      <c r="N7" s="140"/>
+      <c r="O7" s="140"/>
+      <c r="P7" s="140"/>
+      <c r="Q7" s="140"/>
+      <c r="R7" s="140"/>
+      <c r="S7" s="140"/>
       <c r="T7" s="3"/>
       <c r="W7" s="55" t="s">
         <v>4</v>
@@ -7334,7 +7334,7 @@
       </c>
       <c r="E8" s="49"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="145" t="s">
+      <c r="G8" s="141" t="s">
         <v>135</v>
       </c>
       <c r="H8" s="13">
@@ -7432,7 +7432,7 @@
       </c>
       <c r="E9" s="50"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="145"/>
+      <c r="G9" s="141"/>
       <c r="H9" s="13">
         <v>0.7</v>
       </c>
@@ -7528,7 +7528,7 @@
       </c>
       <c r="E10" s="50"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="145"/>
+      <c r="G10" s="141"/>
       <c r="H10" s="13">
         <v>0.65</v>
       </c>
@@ -7624,7 +7624,7 @@
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="145"/>
+      <c r="G11" s="141"/>
       <c r="H11" s="13">
         <v>0.6</v>
       </c>
@@ -7716,7 +7716,7 @@
       <c r="D12" s="51"/>
       <c r="E12" s="51"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="145"/>
+      <c r="G12" s="141"/>
       <c r="H12" s="13">
         <v>0.55000000000000004</v>
       </c>
@@ -7808,7 +7808,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="145"/>
+      <c r="G13" s="141"/>
       <c r="H13" s="13">
         <v>0.5</v>
       </c>
@@ -7902,7 +7902,7 @@
       <c r="D14" s="24"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="145"/>
+      <c r="G14" s="141"/>
       <c r="H14" s="13">
         <v>0.45</v>
       </c>
@@ -7990,13 +7990,13 @@
     </row>
     <row r="15" spans="2:34" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
-      <c r="C15" s="148" t="s">
+      <c r="C15" s="142" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="149"/>
+      <c r="D15" s="143"/>
       <c r="E15" s="48"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="145"/>
+      <c r="G15" s="141"/>
       <c r="H15" s="13">
         <v>0.4</v>
       </c>
@@ -8084,11 +8084,11 @@
     </row>
     <row r="16" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
-      <c r="C16" s="150"/>
-      <c r="D16" s="149"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="143"/>
       <c r="E16" s="48"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="145"/>
+      <c r="G16" s="141"/>
       <c r="H16" s="13">
         <v>0.35</v>
       </c>
@@ -8176,13 +8176,13 @@
     </row>
     <row r="17" spans="2:34" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
-      <c r="C17" s="151" t="s">
+      <c r="C17" s="145" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="152"/>
+      <c r="D17" s="146"/>
       <c r="E17" s="36"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="145"/>
+      <c r="G17" s="141"/>
       <c r="H17" s="13">
         <v>0.3</v>
       </c>
@@ -8270,13 +8270,13 @@
     </row>
     <row r="18" spans="2:34" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
-      <c r="C18" s="151" t="s">
+      <c r="C18" s="145" t="s">
         <v>133</v>
       </c>
-      <c r="D18" s="152"/>
+      <c r="D18" s="146"/>
       <c r="E18" s="36"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="145"/>
+      <c r="G18" s="141"/>
       <c r="H18" s="13">
         <v>0.25</v>
       </c>
@@ -8364,8 +8364,8 @@
     </row>
     <row r="19" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
-      <c r="C19" s="153"/>
-      <c r="D19" s="152"/>
+      <c r="C19" s="147"/>
+      <c r="D19" s="146"/>
       <c r="E19" s="36"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -8443,25 +8443,25 @@
     </row>
     <row r="20" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
-      <c r="C20" s="153"/>
-      <c r="D20" s="152"/>
+      <c r="C20" s="147"/>
+      <c r="D20" s="146"/>
       <c r="E20" s="36"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="139" t="s">
+      <c r="I20" s="150" t="s">
         <v>134</v>
       </c>
-      <c r="J20" s="139"/>
-      <c r="K20" s="139"/>
-      <c r="L20" s="139"/>
-      <c r="M20" s="139"/>
-      <c r="N20" s="139"/>
-      <c r="O20" s="139"/>
-      <c r="P20" s="139"/>
-      <c r="Q20" s="139"/>
-      <c r="R20" s="139"/>
-      <c r="S20" s="139"/>
+      <c r="J20" s="150"/>
+      <c r="K20" s="150"/>
+      <c r="L20" s="150"/>
+      <c r="M20" s="150"/>
+      <c r="N20" s="150"/>
+      <c r="O20" s="150"/>
+      <c r="P20" s="150"/>
+      <c r="Q20" s="150"/>
+      <c r="R20" s="150"/>
+      <c r="S20" s="150"/>
       <c r="T20" s="3"/>
       <c r="W20" s="56">
         <v>0.01</v>
@@ -8502,8 +8502,8 @@
     </row>
     <row r="21" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
-      <c r="C21" s="153"/>
-      <c r="D21" s="152"/>
+      <c r="C21" s="147"/>
+      <c r="D21" s="146"/>
       <c r="E21" s="36"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -8561,8 +8561,8 @@
     </row>
     <row r="22" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
-      <c r="C22" s="154"/>
-      <c r="D22" s="155"/>
+      <c r="C22" s="148"/>
+      <c r="D22" s="149"/>
       <c r="E22" s="36"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -8742,20 +8742,20 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="142" t="str">
+      <c r="I25" s="153" t="str">
         <f>_xlfn.CONCAT("Figure 2. Estimated Number of Severe Fetal Outcomes Under all Possible Immunity and Infection Rate Scenarios, based on ",D8," Pregnancies")</f>
         <v>Figure 2. Estimated Number of Severe Fetal Outcomes Under all Possible Immunity and Infection Rate Scenarios, based on 3600000 Pregnancies</v>
       </c>
-      <c r="J25" s="142"/>
-      <c r="K25" s="142"/>
-      <c r="L25" s="142"/>
-      <c r="M25" s="142"/>
-      <c r="N25" s="142"/>
-      <c r="O25" s="142"/>
-      <c r="P25" s="142"/>
-      <c r="Q25" s="142"/>
-      <c r="R25" s="142"/>
-      <c r="S25" s="142"/>
+      <c r="J25" s="153"/>
+      <c r="K25" s="153"/>
+      <c r="L25" s="153"/>
+      <c r="M25" s="153"/>
+      <c r="N25" s="153"/>
+      <c r="O25" s="153"/>
+      <c r="P25" s="153"/>
+      <c r="Q25" s="153"/>
+      <c r="R25" s="153"/>
+      <c r="S25" s="153"/>
       <c r="T25" s="3"/>
       <c r="W25" s="56">
         <v>0.01</v>
@@ -8796,25 +8796,25 @@
     </row>
     <row r="26" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
-      <c r="C26" s="144" t="s">
+      <c r="C26" s="155" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="144"/>
+      <c r="D26" s="155"/>
       <c r="E26" s="48"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="143"/>
-      <c r="J26" s="143"/>
-      <c r="K26" s="143"/>
-      <c r="L26" s="143"/>
-      <c r="M26" s="143"/>
-      <c r="N26" s="143"/>
-      <c r="O26" s="143"/>
-      <c r="P26" s="143"/>
-      <c r="Q26" s="143"/>
-      <c r="R26" s="143"/>
-      <c r="S26" s="143"/>
+      <c r="I26" s="154"/>
+      <c r="J26" s="154"/>
+      <c r="K26" s="154"/>
+      <c r="L26" s="154"/>
+      <c r="M26" s="154"/>
+      <c r="N26" s="154"/>
+      <c r="O26" s="154"/>
+      <c r="P26" s="154"/>
+      <c r="Q26" s="154"/>
+      <c r="R26" s="154"/>
+      <c r="S26" s="154"/>
       <c r="T26" s="3"/>
       <c r="W26" s="56">
         <v>0.01</v>
@@ -8855,11 +8855,11 @@
     </row>
     <row r="27" spans="2:34" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
-      <c r="C27" s="144"/>
-      <c r="D27" s="144"/>
+      <c r="C27" s="155"/>
+      <c r="D27" s="155"/>
       <c r="E27" s="48"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="145" t="s">
+      <c r="G27" s="141" t="s">
         <v>135</v>
       </c>
       <c r="H27" s="13">
@@ -8949,11 +8949,11 @@
     </row>
     <row r="28" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="3"/>
-      <c r="C28" s="144"/>
-      <c r="D28" s="144"/>
+      <c r="C28" s="155"/>
+      <c r="D28" s="155"/>
       <c r="E28" s="48"/>
       <c r="F28" s="35"/>
-      <c r="G28" s="145"/>
+      <c r="G28" s="141"/>
       <c r="H28" s="13">
         <v>0.9</v>
       </c>
@@ -9041,13 +9041,13 @@
     </row>
     <row r="29" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="3"/>
-      <c r="C29" s="144" t="s">
+      <c r="C29" s="155" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="144"/>
+      <c r="D29" s="155"/>
       <c r="E29" s="48"/>
       <c r="F29" s="35"/>
-      <c r="G29" s="145"/>
+      <c r="G29" s="141"/>
       <c r="H29" s="13">
         <v>0.8</v>
       </c>
@@ -9135,11 +9135,11 @@
     </row>
     <row r="30" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="35"/>
-      <c r="C30" s="144"/>
-      <c r="D30" s="144"/>
+      <c r="C30" s="155"/>
+      <c r="D30" s="155"/>
       <c r="E30" s="48"/>
       <c r="F30" s="35"/>
-      <c r="G30" s="145"/>
+      <c r="G30" s="141"/>
       <c r="H30" s="13">
         <v>0.7</v>
       </c>
@@ -9227,13 +9227,13 @@
     </row>
     <row r="31" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="3"/>
-      <c r="C31" s="144" t="s">
+      <c r="C31" s="155" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="144"/>
+      <c r="D31" s="155"/>
       <c r="E31" s="48"/>
       <c r="F31" s="35"/>
-      <c r="G31" s="145"/>
+      <c r="G31" s="141"/>
       <c r="H31" s="13">
         <v>0.6</v>
       </c>
@@ -9321,11 +9321,11 @@
     </row>
     <row r="32" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="35"/>
-      <c r="C32" s="144"/>
-      <c r="D32" s="144"/>
+      <c r="C32" s="155"/>
+      <c r="D32" s="155"/>
       <c r="E32" s="48"/>
       <c r="F32" s="35"/>
-      <c r="G32" s="145"/>
+      <c r="G32" s="141"/>
       <c r="H32" s="13">
         <v>0.5</v>
       </c>
@@ -9413,13 +9413,13 @@
     </row>
     <row r="33" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="35"/>
-      <c r="C33" s="144" t="s">
+      <c r="C33" s="155" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="144"/>
+      <c r="D33" s="155"/>
       <c r="E33" s="48"/>
       <c r="F33" s="35"/>
-      <c r="G33" s="145"/>
+      <c r="G33" s="141"/>
       <c r="H33" s="13">
         <v>0.4</v>
       </c>
@@ -9507,11 +9507,11 @@
     </row>
     <row r="34" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="35"/>
-      <c r="C34" s="144"/>
-      <c r="D34" s="144"/>
+      <c r="C34" s="155"/>
+      <c r="D34" s="155"/>
       <c r="E34" s="48"/>
       <c r="F34" s="35"/>
-      <c r="G34" s="145"/>
+      <c r="G34" s="141"/>
       <c r="H34" s="13">
         <v>0.3</v>
       </c>
@@ -9599,13 +9599,13 @@
     </row>
     <row r="35" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="35"/>
-      <c r="C35" s="144" t="s">
+      <c r="C35" s="155" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="144"/>
+      <c r="D35" s="155"/>
       <c r="E35" s="48"/>
       <c r="F35" s="35"/>
-      <c r="G35" s="145"/>
+      <c r="G35" s="141"/>
       <c r="H35" s="13">
         <v>0.2</v>
       </c>
@@ -9693,11 +9693,11 @@
     </row>
     <row r="36" spans="2:34" s="8" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="35"/>
-      <c r="C36" s="144"/>
-      <c r="D36" s="144"/>
+      <c r="C36" s="155"/>
+      <c r="D36" s="155"/>
       <c r="E36" s="48"/>
       <c r="F36" s="35"/>
-      <c r="G36" s="145"/>
+      <c r="G36" s="141"/>
       <c r="H36" s="13">
         <v>0.1</v>
       </c>
@@ -9789,7 +9789,7 @@
       <c r="D37" s="35"/>
       <c r="E37" s="35"/>
       <c r="F37" s="35"/>
-      <c r="G37" s="145"/>
+      <c r="G37" s="141"/>
       <c r="H37" s="13">
         <v>0</v>
       </c>
@@ -9962,19 +9962,19 @@
       <c r="F39" s="35"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="139" t="s">
+      <c r="I39" s="150" t="s">
         <v>134</v>
       </c>
-      <c r="J39" s="139"/>
-      <c r="K39" s="139"/>
-      <c r="L39" s="139"/>
-      <c r="M39" s="139"/>
-      <c r="N39" s="139"/>
-      <c r="O39" s="139"/>
-      <c r="P39" s="139"/>
-      <c r="Q39" s="139"/>
-      <c r="R39" s="139"/>
-      <c r="S39" s="139"/>
+      <c r="J39" s="150"/>
+      <c r="K39" s="150"/>
+      <c r="L39" s="150"/>
+      <c r="M39" s="150"/>
+      <c r="N39" s="150"/>
+      <c r="O39" s="150"/>
+      <c r="P39" s="150"/>
+      <c r="Q39" s="150"/>
+      <c r="R39" s="150"/>
+      <c r="S39" s="150"/>
       <c r="T39" s="3"/>
       <c r="W39" s="56">
         <v>0.02</v>
@@ -11139,7 +11139,7 @@
       </c>
     </row>
     <row r="68" spans="14:34" x14ac:dyDescent="0.2">
-      <c r="N68" s="140"/>
+      <c r="N68" s="151"/>
       <c r="O68" s="10"/>
       <c r="P68" s="11"/>
       <c r="Q68" s="11"/>
@@ -11184,7 +11184,7 @@
       </c>
     </row>
     <row r="69" spans="14:34" x14ac:dyDescent="0.2">
-      <c r="N69" s="140"/>
+      <c r="N69" s="151"/>
       <c r="O69" s="10"/>
       <c r="P69" s="11"/>
       <c r="Q69" s="11"/>
@@ -11229,7 +11229,7 @@
       </c>
     </row>
     <row r="70" spans="14:34" x14ac:dyDescent="0.2">
-      <c r="N70" s="140"/>
+      <c r="N70" s="151"/>
       <c r="O70" s="10"/>
       <c r="P70" s="11"/>
       <c r="Q70" s="11"/>
@@ -11274,7 +11274,7 @@
       </c>
     </row>
     <row r="71" spans="14:34" x14ac:dyDescent="0.2">
-      <c r="N71" s="140"/>
+      <c r="N71" s="151"/>
       <c r="O71" s="10"/>
       <c r="P71" s="11"/>
       <c r="Q71" s="11"/>
@@ -11319,7 +11319,7 @@
       </c>
     </row>
     <row r="72" spans="14:34" x14ac:dyDescent="0.2">
-      <c r="N72" s="140"/>
+      <c r="N72" s="151"/>
       <c r="O72" s="10"/>
       <c r="P72" s="11"/>
       <c r="Q72" s="11"/>
@@ -11407,11 +11407,11 @@
       </c>
     </row>
     <row r="74" spans="14:34" x14ac:dyDescent="0.2">
-      <c r="P74" s="141"/>
-      <c r="Q74" s="141"/>
-      <c r="R74" s="141"/>
-      <c r="S74" s="141"/>
-      <c r="T74" s="141"/>
+      <c r="P74" s="152"/>
+      <c r="Q74" s="152"/>
+      <c r="R74" s="152"/>
+      <c r="S74" s="152"/>
+      <c r="T74" s="152"/>
       <c r="W74" s="56">
         <v>0.06</v>
       </c>
@@ -13503,13 +13503,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C3:S3"/>
-    <mergeCell ref="I6:S7"/>
-    <mergeCell ref="G8:G18"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D22"/>
-    <mergeCell ref="I20:S20"/>
     <mergeCell ref="I39:S39"/>
     <mergeCell ref="N68:N72"/>
     <mergeCell ref="P74:T74"/>
@@ -13520,6 +13513,13 @@
     <mergeCell ref="C31:D32"/>
     <mergeCell ref="C33:D34"/>
     <mergeCell ref="C35:D36"/>
+    <mergeCell ref="C3:S3"/>
+    <mergeCell ref="I6:S7"/>
+    <mergeCell ref="G8:G18"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D22"/>
+    <mergeCell ref="I20:S20"/>
   </mergeCells>
   <conditionalFormatting sqref="I8:S18">
     <cfRule type="colorScale" priority="1">
@@ -14673,17 +14673,17 @@
     <row r="10" spans="2:13" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="130" t="s">
+      <c r="D10" s="129" t="s">
         <v>137</v>
       </c>
-      <c r="E10" s="130"/>
-      <c r="F10" s="130"/>
-      <c r="G10" s="130"/>
-      <c r="H10" s="130"/>
-      <c r="I10" s="130"/>
-      <c r="J10" s="130"/>
-      <c r="K10" s="130"/>
-      <c r="L10" s="130"/>
+      <c r="E10" s="129"/>
+      <c r="F10" s="129"/>
+      <c r="G10" s="129"/>
+      <c r="H10" s="129"/>
+      <c r="I10" s="129"/>
+      <c r="J10" s="129"/>
+      <c r="K10" s="129"/>
+      <c r="L10" s="129"/>
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
@@ -14703,17 +14703,17 @@
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="130" t="s">
+      <c r="D12" s="129" t="s">
         <v>102</v>
       </c>
-      <c r="E12" s="130"/>
-      <c r="F12" s="130"/>
-      <c r="G12" s="130"/>
-      <c r="H12" s="130"/>
-      <c r="I12" s="130"/>
-      <c r="J12" s="130"/>
-      <c r="K12" s="130"/>
-      <c r="L12" s="130"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="129"/>
+      <c r="G12" s="129"/>
+      <c r="H12" s="129"/>
+      <c r="I12" s="129"/>
+      <c r="J12" s="129"/>
+      <c r="K12" s="129"/>
+      <c r="L12" s="129"/>
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
@@ -14733,17 +14733,17 @@
     <row r="14" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="130" t="s">
+      <c r="D14" s="129" t="s">
         <v>138</v>
       </c>
-      <c r="E14" s="130"/>
-      <c r="F14" s="130"/>
-      <c r="G14" s="130"/>
-      <c r="H14" s="130"/>
-      <c r="I14" s="130"/>
-      <c r="J14" s="130"/>
-      <c r="K14" s="130"/>
-      <c r="L14" s="130"/>
+      <c r="E14" s="129"/>
+      <c r="F14" s="129"/>
+      <c r="G14" s="129"/>
+      <c r="H14" s="129"/>
+      <c r="I14" s="129"/>
+      <c r="J14" s="129"/>
+      <c r="K14" s="129"/>
+      <c r="L14" s="129"/>
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
@@ -14763,17 +14763,17 @@
     <row r="16" spans="2:13" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="130" t="s">
+      <c r="D16" s="129" t="s">
         <v>139</v>
       </c>
-      <c r="E16" s="130"/>
-      <c r="F16" s="130"/>
-      <c r="G16" s="130"/>
-      <c r="H16" s="130"/>
-      <c r="I16" s="130"/>
-      <c r="J16" s="130"/>
-      <c r="K16" s="130"/>
-      <c r="L16" s="130"/>
+      <c r="E16" s="129"/>
+      <c r="F16" s="129"/>
+      <c r="G16" s="129"/>
+      <c r="H16" s="129"/>
+      <c r="I16" s="129"/>
+      <c r="J16" s="129"/>
+      <c r="K16" s="129"/>
+      <c r="L16" s="129"/>
       <c r="M16" s="3"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
@@ -14793,17 +14793,17 @@
     <row r="18" spans="2:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="130" t="s">
+      <c r="D18" s="129" t="s">
         <v>98</v>
       </c>
-      <c r="E18" s="130"/>
-      <c r="F18" s="130"/>
-      <c r="G18" s="130"/>
-      <c r="H18" s="130"/>
-      <c r="I18" s="130"/>
-      <c r="J18" s="130"/>
-      <c r="K18" s="130"/>
-      <c r="L18" s="130"/>
+      <c r="E18" s="129"/>
+      <c r="F18" s="129"/>
+      <c r="G18" s="129"/>
+      <c r="H18" s="129"/>
+      <c r="I18" s="129"/>
+      <c r="J18" s="129"/>
+      <c r="K18" s="129"/>
+      <c r="L18" s="129"/>
       <c r="M18" s="3"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
@@ -14823,17 +14823,17 @@
     <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="130" t="s">
+      <c r="D20" s="129" t="s">
         <v>140</v>
       </c>
-      <c r="E20" s="130"/>
-      <c r="F20" s="130"/>
-      <c r="G20" s="130"/>
-      <c r="H20" s="130"/>
-      <c r="I20" s="130"/>
-      <c r="J20" s="130"/>
-      <c r="K20" s="130"/>
-      <c r="L20" s="130"/>
+      <c r="E20" s="129"/>
+      <c r="F20" s="129"/>
+      <c r="G20" s="129"/>
+      <c r="H20" s="129"/>
+      <c r="I20" s="129"/>
+      <c r="J20" s="129"/>
+      <c r="K20" s="129"/>
+      <c r="L20" s="129"/>
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
@@ -14883,17 +14883,17 @@
     <row r="24" spans="2:13" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="130" t="s">
+      <c r="D24" s="129" t="s">
         <v>141</v>
       </c>
-      <c r="E24" s="130"/>
-      <c r="F24" s="130"/>
-      <c r="G24" s="130"/>
-      <c r="H24" s="130"/>
-      <c r="I24" s="130"/>
-      <c r="J24" s="130"/>
-      <c r="K24" s="130"/>
-      <c r="L24" s="130"/>
+      <c r="E24" s="129"/>
+      <c r="F24" s="129"/>
+      <c r="G24" s="129"/>
+      <c r="H24" s="129"/>
+      <c r="I24" s="129"/>
+      <c r="J24" s="129"/>
+      <c r="K24" s="129"/>
+      <c r="L24" s="129"/>
       <c r="M24" s="3"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
@@ -14913,17 +14913,17 @@
     <row r="26" spans="2:13" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="130" t="s">
+      <c r="D26" s="129" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="130"/>
-      <c r="F26" s="130"/>
-      <c r="G26" s="130"/>
-      <c r="H26" s="130"/>
-      <c r="I26" s="130"/>
-      <c r="J26" s="130"/>
-      <c r="K26" s="130"/>
-      <c r="L26" s="130"/>
+      <c r="E26" s="129"/>
+      <c r="F26" s="129"/>
+      <c r="G26" s="129"/>
+      <c r="H26" s="129"/>
+      <c r="I26" s="129"/>
+      <c r="J26" s="129"/>
+      <c r="K26" s="129"/>
+      <c r="L26" s="129"/>
       <c r="M26" s="3"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
@@ -14943,17 +14943,17 @@
     <row r="28" spans="2:13" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="130" t="s">
+      <c r="D28" s="129" t="s">
         <v>99</v>
       </c>
-      <c r="E28" s="130"/>
-      <c r="F28" s="130"/>
-      <c r="G28" s="130"/>
-      <c r="H28" s="130"/>
-      <c r="I28" s="130"/>
-      <c r="J28" s="130"/>
-      <c r="K28" s="130"/>
-      <c r="L28" s="130"/>
+      <c r="E28" s="129"/>
+      <c r="F28" s="129"/>
+      <c r="G28" s="129"/>
+      <c r="H28" s="129"/>
+      <c r="I28" s="129"/>
+      <c r="J28" s="129"/>
+      <c r="K28" s="129"/>
+      <c r="L28" s="129"/>
       <c r="M28" s="3"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
@@ -14973,17 +14973,17 @@
     <row r="30" spans="2:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="130" t="s">
+      <c r="D30" s="129" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="130"/>
-      <c r="F30" s="130"/>
-      <c r="G30" s="130"/>
-      <c r="H30" s="130"/>
-      <c r="I30" s="130"/>
-      <c r="J30" s="130"/>
-      <c r="K30" s="130"/>
-      <c r="L30" s="130"/>
+      <c r="E30" s="129"/>
+      <c r="F30" s="129"/>
+      <c r="G30" s="129"/>
+      <c r="H30" s="129"/>
+      <c r="I30" s="129"/>
+      <c r="J30" s="129"/>
+      <c r="K30" s="129"/>
+      <c r="L30" s="129"/>
       <c r="M30" s="3"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
@@ -15058,6 +15058,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C5:L5"/>
+    <mergeCell ref="D20:L20"/>
+    <mergeCell ref="D8:L8"/>
+    <mergeCell ref="D10:L10"/>
+    <mergeCell ref="D26:L26"/>
     <mergeCell ref="D30:L30"/>
     <mergeCell ref="D14:L14"/>
     <mergeCell ref="D12:L12"/>
@@ -15065,11 +15070,6 @@
     <mergeCell ref="D16:L16"/>
     <mergeCell ref="D24:L24"/>
     <mergeCell ref="D28:L28"/>
-    <mergeCell ref="C5:L5"/>
-    <mergeCell ref="D20:L20"/>
-    <mergeCell ref="D8:L8"/>
-    <mergeCell ref="D10:L10"/>
-    <mergeCell ref="D26:L26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>